<commit_message>
prep new data 2024
</commit_message>
<xml_diff>
--- a/new_ghg_series_upload_DCS.xlsx
+++ b/new_ghg_series_upload_DCS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldbankgroup-my.sharepoint.com/personal/tbenschop_worldbank_org/Documents/Documents/GitHub/WDI_GHG_emissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{5518B13A-5684-4547-BCE6-C20F86538A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB8C348C-C590-495F-9877-97D938A53FEA}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{5518B13A-5684-4547-BCE6-C20F86538A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EACDE0AC-2D85-4A36-A119-4F1F1CA8F286}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{29FB456F-6338-4572-9D06-F5CC53B4F8AA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="114">
   <si>
     <t>Code</t>
   </si>
@@ -327,6 +327,57 @@
   </si>
   <si>
     <t>TOTAL('EN.GHG.FGAS.IP.MT.CE.AR5')</t>
+  </si>
+  <si>
+    <t>EN.GHG.ALL.PC.CE.AR5</t>
+  </si>
+  <si>
+    <t>Total greenhouse gas emissions per capita excluding LULUCF (t CO2e/capita)</t>
+  </si>
+  <si>
+    <t>EN.GHG.CO2.PC.CE.AR5</t>
+  </si>
+  <si>
+    <t>Carbon dioxide (CO2) emissions excluding LULUCF per capita (t CO2e/capita)</t>
+  </si>
+  <si>
+    <t>EN.GHG.TOT.ZG.AR5</t>
+  </si>
+  <si>
+    <t>Total greenhouse gas emissions excluding LULUCF (% change from 1990)</t>
+  </si>
+  <si>
+    <t>EN.GHG.CO2.ZG.AR5</t>
+  </si>
+  <si>
+    <t>Carbon dioxide (CO2) emissions (total) excluding LULUCF (% change from 1990)</t>
+  </si>
+  <si>
+    <t>EN.GHG.CH4.ZG.AR5</t>
+  </si>
+  <si>
+    <t>Methane (CH4) emissions (total) excluding LULUCF (% change from 1990)</t>
+  </si>
+  <si>
+    <t>EN.GHG.N2O.ZG.AR5</t>
+  </si>
+  <si>
+    <t>Nitrous oxide (N2O) emissions (total) excluding LULUCF (% change from 1990)</t>
+  </si>
+  <si>
+    <t>EN.GHG.CO2.RT.GDP.KD</t>
+  </si>
+  <si>
+    <t>Carbon intensity of GDP (kg CO2e per 2021 US$ of GDP)</t>
+  </si>
+  <si>
+    <t>EN.GHG.CO2.RT.GDP.PP.KD</t>
+  </si>
+  <si>
+    <t>Carbon intensity of GDP (kg CO2e per 2021 PPP $)</t>
+  </si>
+  <si>
+    <t>Basic</t>
   </si>
 </sst>
 </file>
@@ -707,10 +758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5ACFC7E-347D-4372-A785-2B4D024EE845}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1246,6 +1297,118 @@
         <v>67</v>
       </c>
     </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>97</v>
+      </c>
+      <c r="B31" t="s">
+        <v>98</v>
+      </c>
+      <c r="C31" t="s">
+        <v>66</v>
+      </c>
+      <c r="G31" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" t="s">
+        <v>100</v>
+      </c>
+      <c r="C32" t="s">
+        <v>66</v>
+      </c>
+      <c r="G32" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" t="s">
+        <v>102</v>
+      </c>
+      <c r="C33" t="s">
+        <v>66</v>
+      </c>
+      <c r="G33" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>103</v>
+      </c>
+      <c r="B34" t="s">
+        <v>104</v>
+      </c>
+      <c r="C34" t="s">
+        <v>66</v>
+      </c>
+      <c r="G34" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>105</v>
+      </c>
+      <c r="B35" t="s">
+        <v>106</v>
+      </c>
+      <c r="C35" t="s">
+        <v>66</v>
+      </c>
+      <c r="G35" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>107</v>
+      </c>
+      <c r="B36" t="s">
+        <v>108</v>
+      </c>
+      <c r="C36" t="s">
+        <v>66</v>
+      </c>
+      <c r="G36" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>109</v>
+      </c>
+      <c r="B37" t="s">
+        <v>110</v>
+      </c>
+      <c r="C37" t="s">
+        <v>66</v>
+      </c>
+      <c r="G37" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>111</v>
+      </c>
+      <c r="B38" t="s">
+        <v>112</v>
+      </c>
+      <c r="C38" t="s">
+        <v>66</v>
+      </c>
+      <c r="G38" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>